<commit_message>
Modificado excel de datos
</commit_message>
<xml_diff>
--- a/SeguimientoCartera/_datos.xlsx
+++ b/SeguimientoCartera/_datos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER_MOVIMIENTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="159">
   <si>
     <t>iShares UltraHQ EurGovtBdIdx(IE)InstAcc€</t>
   </si>
@@ -389,18 +389,12 @@
     <t>MERCADO</t>
   </si>
   <si>
-    <t>My Investor</t>
-  </si>
-  <si>
     <t>Degiro</t>
   </si>
   <si>
     <t>Xetra</t>
   </si>
   <si>
-    <t>Self Bank</t>
-  </si>
-  <si>
     <t>COMERCIALIZADOR</t>
   </si>
   <si>
@@ -498,6 +492,18 @@
   </si>
   <si>
     <t>G/P por tipo activo:</t>
+  </si>
+  <si>
+    <t>iShares Eur GovInfLkd BdIdx(IE)InstlAcc€</t>
+  </si>
+  <si>
+    <t>OpenBank</t>
+  </si>
+  <si>
+    <t>MyInvestor</t>
+  </si>
+  <si>
+    <t>SelfBank</t>
   </si>
 </sst>
 </file>
@@ -877,11 +883,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L70"/>
+  <dimension ref="B1:L73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -903,22 +907,22 @@
     <row r="1" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>110</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>29</v>
@@ -927,10 +931,10 @@
         <v>30</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>119</v>
@@ -938,33 +942,33 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="3">
-        <v>44224</v>
+        <v>44225</v>
       </c>
       <c r="F3" s="2">
-        <v>109.81</v>
+        <v>72.75</v>
       </c>
       <c r="G3" s="2">
-        <v>22.3261</v>
+        <v>13.746</v>
       </c>
       <c r="H3" s="2">
         <v>0</v>
       </c>
       <c r="I3" s="4">
-        <v>2451.63</v>
+        <v>1000.02</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J34" si="0">ROUND((F3*G3)+H3,2)</f>
-        <v>2451.63</v>
+        <f t="shared" ref="J3:J5" si="0">ROUND((F3*G3)+H3,2)</f>
+        <v>1000.02</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>56</v>
@@ -972,33 +976,33 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="3">
-        <v>44224</v>
+        <v>44225</v>
       </c>
       <c r="F4" s="2">
-        <v>61.12</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="G4" s="2">
-        <v>35.960299999999997</v>
+        <v>228.71080000000001</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <v>2197.89</v>
+        <v>1111.53</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="0"/>
-        <v>2197.89</v>
+        <v>1111.53</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>56</v>
@@ -1006,33 +1010,33 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="3">
-        <v>44224</v>
+        <v>44225</v>
       </c>
       <c r="F5" s="2">
-        <v>111.95</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="G5" s="2">
-        <v>21.899899999999999</v>
+        <v>227.78100000000001</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="4">
-        <v>2451.69</v>
+        <v>1113.8499999999999</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>2451.69</v>
+        <v>1113.8499999999999</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>56</v>
@@ -1040,33 +1044,33 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="3">
         <v>44224</v>
       </c>
       <c r="F6" s="2">
-        <v>62.39</v>
+        <v>109.81</v>
       </c>
       <c r="G6" s="2">
-        <v>35.234200000000001</v>
+        <v>22.3261</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <v>2198.2600000000002</v>
+        <v>2451.63</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="0"/>
-        <v>2198.2600000000002</v>
+        <f t="shared" ref="J6:J37" si="1">ROUND((F6*G6)+H6,2)</f>
+        <v>2451.63</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>56</v>
@@ -1074,33 +1078,33 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="3">
-        <v>44221</v>
+        <v>44224</v>
       </c>
       <c r="F7" s="2">
-        <v>75.45</v>
+        <v>61.12</v>
       </c>
       <c r="G7" s="2">
-        <v>13.252800000000001</v>
+        <v>35.960299999999997</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
-      <c r="I7" s="2">
-        <v>999.92</v>
+      <c r="I7" s="4">
+        <v>2197.89</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="0"/>
-        <v>999.92</v>
+        <f t="shared" si="1"/>
+        <v>2197.89</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>56</v>
@@ -1108,33 +1112,33 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3">
-        <v>44217</v>
+        <v>44224</v>
       </c>
       <c r="F8" s="2">
-        <v>7.8</v>
+        <v>111.95</v>
       </c>
       <c r="G8" s="2">
-        <v>134.2621</v>
+        <v>21.899899999999999</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
       </c>
       <c r="I8" s="4">
-        <v>1047.24</v>
+        <v>2451.69</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="0"/>
-        <v>1047.24</v>
+        <f t="shared" si="1"/>
+        <v>2451.69</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>56</v>
@@ -1142,67 +1146,67 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" s="3">
-        <v>44216</v>
+        <v>44224</v>
       </c>
       <c r="F9" s="2">
-        <v>10</v>
+        <v>62.39</v>
       </c>
       <c r="G9" s="2">
-        <v>148.19999999999999</v>
+        <v>35.234200000000001</v>
       </c>
       <c r="H9" s="2">
-        <v>2.44</v>
+        <v>0</v>
       </c>
       <c r="I9" s="4">
-        <v>1484.44</v>
+        <v>2198.2600000000002</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="0"/>
-        <v>1484.44</v>
+        <f t="shared" si="1"/>
+        <v>2198.2600000000002</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="3">
-        <v>44215</v>
+        <v>44221</v>
       </c>
       <c r="F10" s="2">
-        <v>7.2629999999999999</v>
+        <v>75.45</v>
       </c>
       <c r="G10" s="2">
-        <v>144.28</v>
+        <v>13.252800000000001</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
       </c>
-      <c r="I10" s="4">
-        <v>1047.9100000000001</v>
+      <c r="I10" s="2">
+        <v>999.92</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="0"/>
-        <v>1047.9100000000001</v>
+        <f t="shared" si="1"/>
+        <v>999.92</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>56</v>
@@ -1210,33 +1214,33 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="3">
-        <v>44200</v>
+        <v>44217</v>
       </c>
       <c r="F11" s="2">
-        <v>4.71</v>
+        <v>7.8</v>
       </c>
       <c r="G11" s="2">
-        <v>236.01429999999999</v>
+        <v>134.2621</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <v>1111.6300000000001</v>
+        <v>1047.24</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="0"/>
-        <v>1111.6300000000001</v>
+        <f t="shared" si="1"/>
+        <v>1047.24</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>56</v>
@@ -1244,67 +1248,67 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="3">
-        <v>44197</v>
+        <v>44216</v>
       </c>
       <c r="F12" s="2">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="G12" s="2">
-        <v>11.46</v>
+        <v>148.19999999999999</v>
       </c>
       <c r="H12" s="2">
-        <v>0</v>
+        <v>2.44</v>
       </c>
       <c r="I12" s="4">
-        <v>1111.6199999999999</v>
+        <v>1484.44</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="0"/>
-        <v>1111.6199999999999</v>
+        <f t="shared" si="1"/>
+        <v>1484.44</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>120</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" s="3">
-        <v>44174</v>
+        <v>44215</v>
       </c>
       <c r="F13" s="2">
-        <v>4.8899999999999997</v>
+        <v>7.2629999999999999</v>
       </c>
       <c r="G13" s="2">
-        <v>217.49080000000001</v>
+        <v>144.28</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
       </c>
       <c r="I13" s="4">
-        <v>1063.53</v>
+        <v>1047.9100000000001</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="0"/>
-        <v>1063.53</v>
+        <f t="shared" si="1"/>
+        <v>1047.9100000000001</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>56</v>
@@ -1312,33 +1316,33 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="3">
-        <v>44174</v>
+        <v>44200</v>
       </c>
       <c r="F14" s="2">
-        <v>4.84</v>
+        <v>4.71</v>
       </c>
       <c r="G14" s="2">
-        <v>219.73830000000001</v>
+        <v>236.01429999999999</v>
       </c>
       <c r="H14" s="2">
         <v>0</v>
       </c>
       <c r="I14" s="4">
-        <v>1063.53</v>
+        <v>1111.6300000000001</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="0"/>
-        <v>1063.53</v>
+        <f t="shared" si="1"/>
+        <v>1111.6300000000001</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>56</v>
@@ -1350,29 +1354,29 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15" s="3">
-        <v>44173</v>
+        <v>44197</v>
       </c>
       <c r="F15" s="2">
         <v>97</v>
       </c>
       <c r="G15" s="2">
-        <v>11.514099999999999</v>
+        <v>11.46</v>
       </c>
       <c r="H15" s="2">
         <v>0</v>
       </c>
       <c r="I15" s="4">
-        <v>1116.8699999999999</v>
+        <v>1111.6199999999999</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="0"/>
-        <v>1116.8699999999999</v>
+        <f t="shared" si="1"/>
+        <v>1111.6199999999999</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>56</v>
@@ -1380,33 +1384,33 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16" s="3">
-        <v>44173</v>
+        <v>44174</v>
       </c>
       <c r="F16" s="2">
-        <v>4.8499999999999996</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="G16" s="2">
-        <v>230.2834</v>
+        <v>217.49080000000001</v>
       </c>
       <c r="H16" s="2">
         <v>0</v>
       </c>
       <c r="I16" s="4">
-        <v>1116.8699999999999</v>
+        <v>1063.53</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="0"/>
-        <v>1116.8699999999999</v>
+        <f t="shared" si="1"/>
+        <v>1063.53</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>56</v>
@@ -1414,33 +1418,33 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E17" s="3">
-        <v>44167</v>
+        <v>44174</v>
       </c>
       <c r="F17" s="2">
-        <v>111.95</v>
+        <v>4.84</v>
       </c>
       <c r="G17" s="2">
-        <v>21.325099999999999</v>
+        <v>219.73830000000001</v>
       </c>
       <c r="H17" s="2">
         <v>0</v>
       </c>
       <c r="I17" s="4">
-        <v>2387.34</v>
+        <v>1063.53</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="0"/>
-        <v>2387.34</v>
+        <f t="shared" si="1"/>
+        <v>1063.53</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>56</v>
@@ -1448,33 +1452,33 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" s="3">
-        <v>44166</v>
+        <v>44173</v>
       </c>
       <c r="F18" s="2">
-        <v>110.08</v>
+        <v>97</v>
       </c>
       <c r="G18" s="2">
-        <v>21.6874</v>
+        <v>11.514099999999999</v>
       </c>
       <c r="H18" s="2">
         <v>0</v>
       </c>
       <c r="I18" s="4">
-        <v>2387.35</v>
+        <v>1116.8699999999999</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="0"/>
-        <v>2387.35</v>
+        <f t="shared" si="1"/>
+        <v>1116.8699999999999</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>56</v>
@@ -1482,33 +1486,33 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E19" s="3">
-        <v>44161</v>
+        <v>44173</v>
       </c>
       <c r="F19" s="2">
-        <v>62.39</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="G19" s="2">
-        <v>34.538899999999998</v>
+        <v>230.2834</v>
       </c>
       <c r="H19" s="2">
         <v>0</v>
       </c>
       <c r="I19" s="4">
-        <v>2154.88</v>
+        <v>1116.8699999999999</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="0"/>
-        <v>2154.88</v>
+        <f t="shared" si="1"/>
+        <v>1116.8699999999999</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>56</v>
@@ -1516,33 +1520,33 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E20" s="3">
-        <v>44160</v>
+        <v>44167</v>
       </c>
       <c r="F20" s="2">
-        <v>61.04</v>
+        <v>111.95</v>
       </c>
       <c r="G20" s="2">
-        <v>35.302700000000002</v>
+        <v>21.325099999999999</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
       </c>
       <c r="I20" s="4">
-        <v>2154.88</v>
+        <v>2387.34</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="0"/>
-        <v>2154.88</v>
+        <f t="shared" si="1"/>
+        <v>2387.34</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>56</v>
@@ -1550,33 +1554,33 @@
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E21" s="3">
-        <v>44159</v>
+        <v>44166</v>
       </c>
       <c r="F21" s="2">
-        <v>11.64</v>
+        <v>110.08</v>
       </c>
       <c r="G21" s="2">
-        <v>189.0292</v>
+        <v>21.6874</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
       </c>
       <c r="I21" s="4">
-        <v>2200.3000000000002</v>
+        <v>2387.35</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="0"/>
-        <v>2200.3000000000002</v>
+        <f t="shared" si="1"/>
+        <v>2387.35</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>56</v>
@@ -1584,33 +1588,33 @@
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E22" s="3">
-        <v>44158</v>
+        <v>44161</v>
       </c>
       <c r="F22" s="2">
-        <v>11.47</v>
+        <v>62.39</v>
       </c>
       <c r="G22" s="2">
-        <v>191.8312</v>
+        <v>34.538899999999998</v>
       </c>
       <c r="H22" s="2">
         <v>0</v>
       </c>
       <c r="I22" s="4">
-        <v>2200.3000000000002</v>
+        <v>2154.88</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" si="0"/>
-        <v>2200.3000000000002</v>
+        <f t="shared" si="1"/>
+        <v>2154.88</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>56</v>
@@ -1618,33 +1622,33 @@
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E23" s="3">
-        <v>44141</v>
+        <v>44160</v>
       </c>
       <c r="F23" s="2">
-        <v>3.7</v>
+        <v>61.04</v>
       </c>
       <c r="G23" s="2">
-        <v>184.09389999999999</v>
+        <v>35.302700000000002</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
       </c>
-      <c r="I23" s="2">
-        <v>681.15</v>
+      <c r="I23" s="4">
+        <v>2154.88</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="0"/>
-        <v>681.15</v>
+        <f t="shared" si="1"/>
+        <v>2154.88</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>56</v>
@@ -1652,33 +1656,33 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E24" s="3">
-        <v>44140</v>
+        <v>44159</v>
       </c>
       <c r="F24" s="2">
-        <v>19.86</v>
+        <v>11.64</v>
       </c>
       <c r="G24" s="2">
-        <v>34.328000000000003</v>
+        <v>189.0292</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
       </c>
-      <c r="I24" s="2">
-        <v>681.75</v>
+      <c r="I24" s="4">
+        <v>2200.3000000000002</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="0"/>
-        <v>681.75</v>
+        <f t="shared" si="1"/>
+        <v>2200.3000000000002</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>56</v>
@@ -1686,33 +1690,33 @@
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E25" s="3">
-        <v>44138</v>
+        <v>44158</v>
       </c>
       <c r="F25" s="2">
-        <v>3.56</v>
+        <v>11.47</v>
       </c>
       <c r="G25" s="2">
-        <v>274.09840000000003</v>
+        <v>191.8312</v>
       </c>
       <c r="H25" s="2">
         <v>0</v>
       </c>
-      <c r="I25" s="2">
-        <v>975.79</v>
+      <c r="I25" s="4">
+        <v>2200.3000000000002</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" si="0"/>
-        <v>975.79</v>
+        <f t="shared" si="1"/>
+        <v>2200.3000000000002</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>56</v>
@@ -1720,33 +1724,33 @@
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E26" s="3">
-        <v>44138</v>
+        <v>44141</v>
       </c>
       <c r="F26" s="2">
-        <v>3.44</v>
+        <v>3.7</v>
       </c>
       <c r="G26" s="2">
-        <v>274.09840000000003</v>
+        <v>184.09389999999999</v>
       </c>
       <c r="H26" s="2">
         <v>0</v>
       </c>
       <c r="I26" s="2">
-        <v>942.9</v>
+        <v>681.15</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="0"/>
-        <v>942.9</v>
+        <f t="shared" si="1"/>
+        <v>681.15</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>56</v>
@@ -1754,33 +1758,33 @@
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="3">
-        <v>44138</v>
+        <v>44140</v>
       </c>
       <c r="F27" s="2">
-        <v>42.28</v>
+        <v>19.86</v>
       </c>
       <c r="G27" s="2">
-        <v>18.919799999999999</v>
+        <v>34.328000000000003</v>
       </c>
       <c r="H27" s="2">
         <v>0</v>
       </c>
       <c r="I27" s="2">
-        <v>799.93</v>
+        <v>681.75</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" si="0"/>
-        <v>799.93</v>
+        <f t="shared" si="1"/>
+        <v>681.75</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>56</v>
@@ -1788,33 +1792,33 @@
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E28" s="3">
-        <v>44137</v>
+        <v>44138</v>
       </c>
       <c r="F28" s="2">
-        <v>73</v>
+        <v>3.56</v>
       </c>
       <c r="G28" s="2">
-        <v>13.381</v>
+        <v>274.09840000000003</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
       </c>
       <c r="I28" s="2">
-        <v>976.81</v>
+        <v>975.79</v>
       </c>
       <c r="J28" s="2">
-        <f t="shared" si="0"/>
-        <v>976.81</v>
+        <f t="shared" si="1"/>
+        <v>975.79</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>56</v>
@@ -1822,33 +1826,33 @@
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E29" s="3">
-        <v>44137</v>
+        <v>44138</v>
       </c>
       <c r="F29" s="2">
-        <v>6.5</v>
+        <v>3.44</v>
       </c>
       <c r="G29" s="2">
-        <v>145.26</v>
+        <v>274.09840000000003</v>
       </c>
       <c r="H29" s="2">
         <v>0</v>
       </c>
       <c r="I29" s="2">
-        <v>944.19</v>
+        <v>942.9</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" si="0"/>
-        <v>944.19</v>
+        <f t="shared" si="1"/>
+        <v>942.9</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>56</v>
@@ -1856,33 +1860,33 @@
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E30" s="3">
-        <v>44132</v>
+        <v>44138</v>
       </c>
       <c r="F30" s="2">
-        <v>150</v>
+        <v>42.28</v>
       </c>
       <c r="G30" s="2">
-        <v>13.311</v>
+        <v>18.919799999999999</v>
       </c>
       <c r="H30" s="2">
         <v>0</v>
       </c>
-      <c r="I30" s="4">
-        <v>1996.65</v>
+      <c r="I30" s="2">
+        <v>799.93</v>
       </c>
       <c r="J30" s="2">
-        <f t="shared" si="0"/>
-        <v>1996.65</v>
+        <f t="shared" si="1"/>
+        <v>799.93</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>56</v>
@@ -1890,33 +1894,33 @@
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E31" s="3">
-        <v>44131</v>
+        <v>44137</v>
       </c>
       <c r="F31" s="2">
-        <v>13.763</v>
+        <v>73</v>
       </c>
       <c r="G31" s="2">
-        <v>145.31</v>
+        <v>13.381</v>
       </c>
       <c r="H31" s="2">
         <v>0</v>
       </c>
-      <c r="I31" s="4">
-        <v>1999.9</v>
+      <c r="I31" s="2">
+        <v>976.81</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="0"/>
-        <v>1999.9</v>
+        <f t="shared" si="1"/>
+        <v>976.81</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>56</v>
@@ -1924,33 +1928,33 @@
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E32" s="3">
-        <v>44131</v>
+        <v>44137</v>
       </c>
       <c r="F32" s="2">
-        <v>3.69</v>
+        <v>6.5</v>
       </c>
       <c r="G32" s="2">
-        <v>270.69080000000002</v>
+        <v>145.26</v>
       </c>
       <c r="H32" s="2">
         <v>0</v>
       </c>
       <c r="I32" s="2">
-        <v>998.85</v>
+        <v>944.19</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="0"/>
-        <v>998.85</v>
+        <f t="shared" si="1"/>
+        <v>944.19</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>56</v>
@@ -1958,104 +1962,104 @@
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E33" s="3">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="F33" s="2">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="G33" s="2">
-        <v>210.8</v>
+        <v>13.311</v>
       </c>
       <c r="H33" s="2">
-        <v>2.89</v>
+        <v>0</v>
       </c>
       <c r="I33" s="4">
-        <v>2948.31</v>
+        <v>1996.65</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="0"/>
-        <v>2954.09</v>
+        <f t="shared" si="1"/>
+        <v>1996.65</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E34" s="3">
-        <v>44127</v>
+        <v>44131</v>
       </c>
       <c r="F34" s="2">
-        <v>31</v>
+        <v>13.763</v>
       </c>
       <c r="G34" s="2">
-        <v>155.5</v>
+        <v>145.31</v>
       </c>
       <c r="H34" s="2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I34" s="4">
-        <v>4835.5</v>
+        <v>1999.9</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="0"/>
-        <v>4835.5</v>
+        <f t="shared" si="1"/>
+        <v>1999.9</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E35" s="3">
-        <v>44127</v>
+        <v>44131</v>
       </c>
       <c r="F35" s="2">
-        <v>19</v>
+        <v>3.69</v>
       </c>
       <c r="G35" s="2">
-        <v>155.56</v>
+        <v>270.69080000000002</v>
       </c>
       <c r="H35" s="2">
         <v>0</v>
       </c>
-      <c r="I35" s="4">
-        <v>2955.64</v>
+      <c r="I35" s="2">
+        <v>998.85</v>
       </c>
       <c r="J35" s="2">
-        <f t="shared" ref="J35:J70" si="1">ROUND((F35*G35)+H35,2)</f>
-        <v>2955.64</v>
+        <f t="shared" si="1"/>
+        <v>998.85</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.2">
@@ -2064,165 +2068,165 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E36" s="3">
-        <v>44118</v>
+        <v>44131</v>
       </c>
       <c r="F36" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G36" s="2">
-        <v>209.24</v>
+        <v>210.8</v>
       </c>
       <c r="H36" s="2">
-        <v>2.25</v>
-      </c>
-      <c r="I36" s="2">
-        <v>839.21</v>
+        <v>2.89</v>
+      </c>
+      <c r="I36" s="4">
+        <v>2948.31</v>
       </c>
       <c r="J36" s="2">
         <f t="shared" si="1"/>
-        <v>839.21</v>
+        <v>2954.09</v>
       </c>
       <c r="K36" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L36" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E37" s="3">
-        <v>44118</v>
+        <v>44127</v>
       </c>
       <c r="F37" s="2">
-        <v>3.37</v>
+        <v>31</v>
       </c>
       <c r="G37" s="2">
-        <v>270.59899999999999</v>
+        <v>155.5</v>
       </c>
       <c r="H37" s="2">
-        <v>2.4700000000000002</v>
-      </c>
-      <c r="I37" s="2">
-        <v>909.45</v>
+        <v>15</v>
+      </c>
+      <c r="I37" s="4">
+        <v>4835.5</v>
       </c>
       <c r="J37" s="2">
         <f t="shared" si="1"/>
-        <v>914.39</v>
+        <v>4835.5</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>120</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E38" s="3">
-        <v>44112</v>
+        <v>44127</v>
       </c>
       <c r="F38" s="2">
-        <v>7.77</v>
+        <v>19</v>
       </c>
       <c r="G38" s="2">
-        <v>173.68</v>
+        <v>155.56</v>
       </c>
       <c r="H38" s="2">
         <v>0</v>
       </c>
       <c r="I38" s="4">
-        <v>1349.49</v>
+        <v>2955.64</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="1"/>
-        <v>1349.49</v>
+        <f t="shared" ref="J38:J73" si="2">ROUND((F38*G38)+H38,2)</f>
+        <v>2955.64</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E39" s="3">
-        <v>44112</v>
+        <v>44118</v>
       </c>
       <c r="F39" s="2">
-        <v>3.77</v>
+        <v>4</v>
       </c>
       <c r="G39" s="2">
-        <v>266.44229999999999</v>
+        <v>209.24</v>
       </c>
       <c r="H39" s="2">
-        <v>0</v>
-      </c>
-      <c r="I39" s="4">
-        <v>1004.49</v>
+        <v>2.25</v>
+      </c>
+      <c r="I39" s="2">
+        <v>839.21</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="1"/>
-        <v>1004.49</v>
+        <f t="shared" si="2"/>
+        <v>839.21</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>120</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E40" s="3">
-        <v>44112</v>
+        <v>44118</v>
       </c>
       <c r="F40" s="2">
-        <v>76</v>
+        <v>3.37</v>
       </c>
       <c r="G40" s="2">
-        <v>13.250999999999999</v>
+        <v>270.59899999999999</v>
       </c>
       <c r="H40" s="2">
-        <v>0</v>
-      </c>
-      <c r="I40" s="4">
-        <v>1007.08</v>
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="I40" s="2">
+        <v>909.45</v>
       </c>
       <c r="J40" s="2">
-        <f t="shared" si="1"/>
-        <v>1007.08</v>
+        <f t="shared" si="2"/>
+        <v>914.39</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="L40" s="2" t="s">
         <v>56</v>
@@ -2230,33 +2234,33 @@
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E41" s="3">
-        <v>44110</v>
+        <v>44112</v>
       </c>
       <c r="F41" s="2">
-        <v>8.93</v>
+        <v>7.77</v>
       </c>
       <c r="G41" s="2">
-        <v>33.03</v>
+        <v>173.68</v>
       </c>
       <c r="H41" s="2">
         <v>0</v>
       </c>
-      <c r="I41" s="2">
-        <v>294.95999999999998</v>
+      <c r="I41" s="4">
+        <v>1349.49</v>
       </c>
       <c r="J41" s="2">
-        <f t="shared" si="1"/>
-        <v>294.95999999999998</v>
+        <f t="shared" si="2"/>
+        <v>1349.49</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="L41" s="2" t="s">
         <v>56</v>
@@ -2264,33 +2268,33 @@
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E42" s="3">
-        <v>44110</v>
+        <v>44112</v>
       </c>
       <c r="F42" s="2">
-        <v>17.5</v>
+        <v>3.77</v>
       </c>
       <c r="G42" s="2">
-        <v>20</v>
+        <v>266.44229999999999</v>
       </c>
       <c r="H42" s="2">
         <v>0</v>
       </c>
-      <c r="I42" s="2">
-        <v>350</v>
+      <c r="I42" s="4">
+        <v>1004.49</v>
       </c>
       <c r="J42" s="2">
-        <f t="shared" si="1"/>
-        <v>350</v>
+        <f t="shared" si="2"/>
+        <v>1004.49</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>56</v>
@@ -2298,271 +2302,271 @@
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E43" s="3">
-        <v>44106</v>
+        <v>44112</v>
       </c>
       <c r="F43" s="2">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="G43" s="2">
-        <v>46.19</v>
+        <v>13.250999999999999</v>
       </c>
       <c r="H43" s="2">
-        <v>2.2999999999999998</v>
+        <v>0</v>
       </c>
       <c r="I43" s="4">
-        <v>1013.88</v>
+        <v>1007.08</v>
       </c>
       <c r="J43" s="2">
-        <f t="shared" si="1"/>
-        <v>1018.48</v>
+        <f t="shared" si="2"/>
+        <v>1007.08</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E44" s="3">
-        <v>44106</v>
+        <v>44110</v>
       </c>
       <c r="F44" s="2">
-        <v>47</v>
+        <v>8.93</v>
       </c>
       <c r="G44" s="2">
-        <v>21.504999999999999</v>
+        <v>33.03</v>
       </c>
       <c r="H44" s="2">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="I44" s="4">
-        <v>1008.44</v>
+        <v>0</v>
+      </c>
+      <c r="I44" s="2">
+        <v>294.95999999999998</v>
       </c>
       <c r="J44" s="2">
-        <f t="shared" si="1"/>
-        <v>1013.04</v>
+        <f t="shared" si="2"/>
+        <v>294.95999999999998</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E45" s="3">
-        <v>44106</v>
+        <v>44110</v>
       </c>
       <c r="F45" s="2">
-        <v>27</v>
+        <v>17.5</v>
       </c>
       <c r="G45" s="2">
-        <v>37.72</v>
+        <v>20</v>
       </c>
       <c r="H45" s="2">
-        <v>2.31</v>
-      </c>
-      <c r="I45" s="4">
-        <v>1016.13</v>
+        <v>0</v>
+      </c>
+      <c r="I45" s="2">
+        <v>350</v>
       </c>
       <c r="J45" s="2">
-        <f t="shared" si="1"/>
-        <v>1020.75</v>
+        <f t="shared" si="2"/>
+        <v>350</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E46" s="3">
-        <v>44105</v>
+        <v>44106</v>
       </c>
       <c r="F46" s="2">
-        <v>4.84</v>
+        <v>22</v>
       </c>
       <c r="G46" s="2">
-        <v>206.73349999999999</v>
+        <v>46.19</v>
       </c>
       <c r="H46" s="2">
-        <v>0</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I46" s="4">
-        <v>1000.59</v>
+        <v>1013.88</v>
       </c>
       <c r="J46" s="2">
-        <f t="shared" si="1"/>
-        <v>1000.59</v>
+        <f t="shared" si="2"/>
+        <v>1018.48</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E47" s="3">
-        <v>44105</v>
+        <v>44106</v>
       </c>
       <c r="F47" s="2">
-        <v>4.8499999999999996</v>
+        <v>47</v>
       </c>
       <c r="G47" s="2">
-        <v>206.06389999999999</v>
+        <v>21.504999999999999</v>
       </c>
       <c r="H47" s="2">
-        <v>0</v>
-      </c>
-      <c r="I47" s="2">
-        <v>999.41</v>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I47" s="4">
+        <v>1008.44</v>
       </c>
       <c r="J47" s="2">
-        <f t="shared" si="1"/>
-        <v>999.41</v>
+        <f t="shared" si="2"/>
+        <v>1013.04</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E48" s="3">
-        <v>44104</v>
+        <v>44106</v>
       </c>
       <c r="F48" s="2">
-        <v>32.25</v>
+        <v>27</v>
       </c>
       <c r="G48" s="2">
-        <v>33.007399999999997</v>
+        <v>37.72</v>
       </c>
       <c r="H48" s="2">
-        <v>0</v>
+        <v>2.31</v>
       </c>
       <c r="I48" s="4">
-        <v>1064.49</v>
+        <v>1016.13</v>
       </c>
       <c r="J48" s="2">
-        <f t="shared" si="1"/>
-        <v>1064.49</v>
+        <f t="shared" si="2"/>
+        <v>1020.75</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E49" s="3">
-        <v>44104</v>
+        <v>44105</v>
       </c>
       <c r="F49" s="2">
-        <v>4</v>
+        <v>4.84</v>
       </c>
       <c r="G49" s="2">
-        <v>284.8</v>
+        <v>206.73349999999999</v>
       </c>
       <c r="H49" s="2">
         <v>0</v>
       </c>
       <c r="I49" s="4">
-        <v>1139.2</v>
+        <v>1000.59</v>
       </c>
       <c r="J49" s="2">
-        <f t="shared" si="1"/>
-        <v>1139.2</v>
+        <f t="shared" si="2"/>
+        <v>1000.59</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E50" s="3">
-        <v>44099</v>
+        <v>44105</v>
       </c>
       <c r="F50" s="2">
-        <v>50.3</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="G50" s="2">
-        <v>19.8811</v>
+        <v>206.06389999999999</v>
       </c>
       <c r="H50" s="2">
         <v>0</v>
       </c>
-      <c r="I50" s="4">
-        <v>1000.02</v>
+      <c r="I50" s="2">
+        <v>999.41</v>
       </c>
       <c r="J50" s="2">
-        <f t="shared" si="1"/>
-        <v>1000.02</v>
+        <f t="shared" si="2"/>
+        <v>999.41</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>56</v>
@@ -2570,449 +2574,449 @@
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E51" s="3">
-        <v>44099</v>
+        <v>44104</v>
       </c>
       <c r="F51" s="2">
-        <v>7</v>
+        <v>32.25</v>
       </c>
       <c r="G51" s="2">
-        <v>147.4</v>
+        <v>33.007399999999997</v>
       </c>
       <c r="H51" s="2">
-        <v>2.31</v>
+        <v>0</v>
       </c>
       <c r="I51" s="4">
-        <v>1029.49</v>
+        <v>1064.49</v>
       </c>
       <c r="J51" s="2">
-        <f t="shared" si="1"/>
-        <v>1034.1099999999999</v>
+        <f t="shared" si="2"/>
+        <v>1064.49</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E52" s="3">
-        <v>44098</v>
+        <v>44104</v>
       </c>
       <c r="F52" s="2">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G52" s="2">
-        <v>266.12259999999998</v>
+        <v>284.8</v>
       </c>
       <c r="H52" s="2">
         <v>0</v>
       </c>
       <c r="I52" s="4">
-        <v>3991.84</v>
+        <v>1139.2</v>
       </c>
       <c r="J52" s="2">
-        <f t="shared" si="1"/>
-        <v>3991.84</v>
+        <f t="shared" si="2"/>
+        <v>1139.2</v>
       </c>
       <c r="K52" s="2" t="s">
         <v>120</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E53" s="3">
-        <v>44098</v>
+        <v>44099</v>
       </c>
       <c r="F53" s="2">
-        <v>19</v>
+        <v>50.3</v>
       </c>
       <c r="G53" s="2">
-        <v>154.05000000000001</v>
+        <v>19.8811</v>
       </c>
       <c r="H53" s="2">
         <v>0</v>
       </c>
       <c r="I53" s="4">
-        <v>2926.95</v>
+        <v>1000.02</v>
       </c>
       <c r="J53" s="2">
-        <f t="shared" si="1"/>
-        <v>2926.95</v>
+        <f t="shared" si="2"/>
+        <v>1000.02</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E54" s="3">
-        <v>44098</v>
+        <v>44099</v>
       </c>
       <c r="F54" s="2">
-        <v>160</v>
+        <v>7</v>
       </c>
       <c r="G54" s="2">
-        <v>6.4565999999999999</v>
+        <v>147.4</v>
       </c>
       <c r="H54" s="2">
         <v>2.31</v>
       </c>
       <c r="I54" s="4">
-        <v>1030.75</v>
+        <v>1029.49</v>
       </c>
       <c r="J54" s="2">
-        <f t="shared" si="1"/>
-        <v>1035.3699999999999</v>
+        <f t="shared" si="2"/>
+        <v>1034.1099999999999</v>
       </c>
       <c r="K54" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L54" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E55" s="3">
         <v>44098</v>
       </c>
       <c r="F55" s="2">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G55" s="2">
-        <v>177.77</v>
+        <v>266.12259999999998</v>
       </c>
       <c r="H55" s="2">
-        <v>2.59</v>
+        <v>0</v>
       </c>
       <c r="I55" s="4">
-        <v>1952.88</v>
+        <v>3991.84</v>
       </c>
       <c r="J55" s="2">
-        <f t="shared" si="1"/>
-        <v>1958.06</v>
+        <f t="shared" si="2"/>
+        <v>3991.84</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E56" s="3">
         <v>44098</v>
       </c>
       <c r="F56" s="2">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G56" s="2">
-        <v>266.1225</v>
+        <v>154.05000000000001</v>
       </c>
       <c r="H56" s="2">
         <v>0</v>
       </c>
       <c r="I56" s="4">
-        <v>1064.49</v>
+        <v>2926.95</v>
       </c>
       <c r="J56" s="2">
-        <f t="shared" si="1"/>
-        <v>1064.49</v>
+        <f t="shared" si="2"/>
+        <v>2926.95</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>120</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E57" s="3">
-        <v>44092</v>
+        <v>44098</v>
       </c>
       <c r="F57" s="2">
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="G57" s="2">
-        <v>13.231999999999999</v>
+        <v>6.4565999999999999</v>
       </c>
       <c r="H57" s="2">
-        <v>0</v>
+        <v>2.31</v>
       </c>
       <c r="I57" s="4">
-        <v>1005.63</v>
+        <v>1030.75</v>
       </c>
       <c r="J57" s="2">
-        <f t="shared" si="1"/>
-        <v>1005.63</v>
+        <f t="shared" si="2"/>
+        <v>1035.3699999999999</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>120</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E58" s="3">
-        <v>44020</v>
+        <v>44098</v>
       </c>
       <c r="F58" s="2">
-        <v>160</v>
+        <v>11</v>
       </c>
       <c r="G58" s="2">
-        <v>6.3238000000000003</v>
+        <v>177.77</v>
       </c>
       <c r="H58" s="2">
-        <v>2.2999999999999998</v>
+        <v>2.59</v>
       </c>
       <c r="I58" s="4">
-        <v>1014.11</v>
+        <v>1952.88</v>
       </c>
       <c r="J58" s="2">
-        <f t="shared" si="1"/>
-        <v>1014.11</v>
+        <f t="shared" si="2"/>
+        <v>1958.06</v>
       </c>
       <c r="K58" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L58" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E59" s="3">
-        <v>44020</v>
+        <v>44098</v>
       </c>
       <c r="F59" s="2">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G59" s="2">
-        <v>47.51</v>
+        <v>266.1225</v>
       </c>
       <c r="H59" s="2">
-        <v>2.31</v>
+        <v>0</v>
       </c>
       <c r="I59" s="4">
-        <v>1047.53</v>
+        <v>1064.49</v>
       </c>
       <c r="J59" s="2">
-        <f t="shared" si="1"/>
-        <v>1047.53</v>
+        <f t="shared" si="2"/>
+        <v>1064.49</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E60" s="3">
-        <v>44020</v>
+        <v>44092</v>
       </c>
       <c r="F60" s="2">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="G60" s="2">
-        <v>21.68</v>
+        <v>13.231999999999999</v>
       </c>
       <c r="H60" s="2">
-        <v>2.31</v>
+        <v>0</v>
       </c>
       <c r="I60" s="4">
-        <v>1021.27</v>
+        <v>1005.63</v>
       </c>
       <c r="J60" s="2">
-        <f t="shared" si="1"/>
-        <v>1021.27</v>
+        <f t="shared" si="2"/>
+        <v>1005.63</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E61" s="3">
-        <v>43998</v>
+        <v>44020</v>
       </c>
       <c r="F61" s="2">
-        <v>7</v>
+        <v>160</v>
       </c>
       <c r="G61" s="2">
-        <v>151.5</v>
+        <v>6.3238000000000003</v>
       </c>
       <c r="H61" s="2">
-        <v>2.3199999999999998</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I61" s="4">
-        <v>1062.82</v>
+        <v>1014.11</v>
       </c>
       <c r="J61" s="2">
-        <f t="shared" si="1"/>
-        <v>1062.82</v>
+        <f t="shared" si="2"/>
+        <v>1014.11</v>
       </c>
       <c r="K61" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L61" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="L61" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E62" s="3">
-        <v>43998</v>
+        <v>44020</v>
       </c>
       <c r="F62" s="2">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="G62" s="2">
-        <v>173.99</v>
+        <v>47.51</v>
       </c>
       <c r="H62" s="2">
         <v>2.31</v>
       </c>
       <c r="I62" s="4">
-        <v>1046.25</v>
+        <v>1047.53</v>
       </c>
       <c r="J62" s="2">
-        <f t="shared" si="1"/>
-        <v>1046.25</v>
+        <f t="shared" si="2"/>
+        <v>1047.53</v>
       </c>
       <c r="K62" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L62" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="L62" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E63" s="3">
-        <v>43998</v>
+        <v>44020</v>
       </c>
       <c r="F63" s="2">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="G63" s="2">
-        <v>202.95</v>
+        <v>21.68</v>
       </c>
       <c r="H63" s="2">
-        <v>2.2999999999999998</v>
+        <v>2.31</v>
       </c>
       <c r="I63" s="4">
-        <v>1017.05</v>
+        <v>1021.27</v>
       </c>
       <c r="J63" s="2">
-        <f t="shared" si="1"/>
-        <v>1017.05</v>
+        <f t="shared" si="2"/>
+        <v>1021.27</v>
       </c>
       <c r="K63" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L63" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="L63" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
@@ -3022,31 +3026,31 @@
         <v>43998</v>
       </c>
       <c r="F64" s="2">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="G64" s="2">
-        <v>37.585000000000001</v>
+        <v>151.5</v>
       </c>
       <c r="H64" s="2">
-        <v>2.2999999999999998</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="I64" s="4">
-        <v>1017.1</v>
+        <v>1062.82</v>
       </c>
       <c r="J64" s="2">
-        <f t="shared" si="1"/>
-        <v>1017.1</v>
+        <f t="shared" si="2"/>
+        <v>1062.82</v>
       </c>
       <c r="K64" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L64" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="L64" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
@@ -3056,196 +3060,298 @@
         <v>43998</v>
       </c>
       <c r="F65" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G65" s="2">
-        <v>279.01</v>
+        <v>173.99</v>
       </c>
       <c r="H65" s="2">
-        <v>2.33</v>
+        <v>2.31</v>
       </c>
       <c r="I65" s="4">
-        <v>1118.3699999999999</v>
+        <v>1046.25</v>
       </c>
       <c r="J65" s="2">
-        <f t="shared" si="1"/>
-        <v>1118.3699999999999</v>
+        <f t="shared" si="2"/>
+        <v>1046.25</v>
       </c>
       <c r="K65" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L65" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="L65" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E66" s="3">
         <v>43998</v>
       </c>
       <c r="F66" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G66" s="2">
-        <v>72.650000000000006</v>
+        <v>202.95</v>
       </c>
       <c r="H66" s="2">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="I66" s="2">
-        <v>942.17</v>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I66" s="4">
+        <v>1017.05</v>
       </c>
       <c r="J66" s="2">
-        <f t="shared" si="1"/>
-        <v>946.73</v>
+        <f t="shared" si="2"/>
+        <v>1017.05</v>
       </c>
       <c r="K66" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L66" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="L66" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B67" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E67" s="3">
-        <v>43992</v>
+        <v>43998</v>
       </c>
       <c r="F67" s="2">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="G67" s="2">
-        <v>73.67</v>
+        <v>37.585000000000001</v>
       </c>
       <c r="H67" s="2">
-        <v>2.29</v>
-      </c>
-      <c r="I67" s="2">
-        <v>960</v>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I67" s="4">
+        <v>1017.1</v>
       </c>
       <c r="J67" s="2">
-        <f t="shared" si="1"/>
-        <v>960</v>
+        <f t="shared" si="2"/>
+        <v>1017.1</v>
       </c>
       <c r="K67" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L67" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="L67" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B68" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E68" s="3">
-        <v>43991</v>
+        <v>43998</v>
       </c>
       <c r="F68" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G68" s="2">
-        <v>199.636</v>
+        <v>279.01</v>
       </c>
       <c r="H68" s="2">
-        <v>2.2999999999999998</v>
+        <v>2.33</v>
       </c>
       <c r="I68" s="4">
-        <v>1000.48</v>
+        <v>1118.3699999999999</v>
       </c>
       <c r="J68" s="2">
-        <f t="shared" si="1"/>
-        <v>1000.48</v>
+        <f t="shared" si="2"/>
+        <v>1118.3699999999999</v>
       </c>
       <c r="K68" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L68" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="L68" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B69" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E69" s="3">
-        <v>43991</v>
+        <v>43998</v>
       </c>
       <c r="F69" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G69" s="2">
-        <v>171.02</v>
+        <v>72.650000000000006</v>
       </c>
       <c r="H69" s="2">
-        <v>2.2599999999999998</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="I69" s="2">
-        <v>857.36</v>
+        <v>942.17</v>
       </c>
       <c r="J69" s="2">
-        <f t="shared" si="1"/>
-        <v>857.36</v>
+        <f t="shared" si="2"/>
+        <v>946.73</v>
       </c>
       <c r="K69" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L69" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="L69" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B70" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E70" s="3">
+        <v>43992</v>
+      </c>
+      <c r="F70" s="2">
+        <v>13</v>
+      </c>
+      <c r="G70" s="2">
+        <v>73.67</v>
+      </c>
+      <c r="H70" s="2">
+        <v>2.29</v>
+      </c>
+      <c r="I70" s="2">
+        <v>960</v>
+      </c>
+      <c r="J70" s="2">
+        <f t="shared" si="2"/>
+        <v>960</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B71" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E71" s="3">
         <v>43991</v>
       </c>
-      <c r="F70" s="2">
+      <c r="F71" s="2">
+        <v>5</v>
+      </c>
+      <c r="G71" s="2">
+        <v>199.636</v>
+      </c>
+      <c r="H71" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I71" s="4">
+        <v>1000.48</v>
+      </c>
+      <c r="J71" s="2">
+        <f t="shared" si="2"/>
+        <v>1000.48</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B72" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" s="3">
+        <v>43991</v>
+      </c>
+      <c r="F72" s="2">
+        <v>5</v>
+      </c>
+      <c r="G72" s="2">
+        <v>171.02</v>
+      </c>
+      <c r="H72" s="2">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="I72" s="2">
+        <v>857.36</v>
+      </c>
+      <c r="J72" s="2">
+        <f t="shared" si="2"/>
+        <v>857.36</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B73" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E73" s="3">
+        <v>43991</v>
+      </c>
+      <c r="F73" s="2">
         <v>61</v>
       </c>
-      <c r="G70" s="2">
+      <c r="G73" s="2">
         <v>48.7</v>
       </c>
-      <c r="H70" s="2">
+      <c r="H73" s="2">
         <v>15</v>
       </c>
-      <c r="I70" s="4">
+      <c r="I73" s="4">
         <v>2985.7</v>
       </c>
-      <c r="J70" s="2">
-        <f t="shared" si="1"/>
+      <c r="J73" s="2">
+        <f t="shared" si="2"/>
         <v>2985.7</v>
       </c>
-      <c r="K70" s="2" t="s">
+      <c r="K73" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L73" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="L70" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -3280,7 +3386,7 @@
     <row r="1" spans="2:10" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>110</v>
@@ -3304,7 +3410,7 @@
         <v>38</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
@@ -4117,19 +4223,19 @@
     <row r="1" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>110</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
@@ -4532,7 +4638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -4556,212 +4662,212 @@
     <row r="1" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>110</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>134</v>
-      </c>
       <c r="H2" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>143</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>119</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>110</v>
       </c>
       <c r="E22" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="I22" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="J22" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K22" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>153</v>
-      </c>
       <c r="L22" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>153</v>
-      </c>
       <c r="G24" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificado fichero SQL y BBDD seguimiento_cartera
</commit_message>
<xml_diff>
--- a/SeguimientoCartera/_datos.xlsx
+++ b/SeguimientoCartera/_datos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="160">
   <si>
     <t>iShares UltraHQ EurGovtBdIdx(IE)InstAcc€</t>
   </si>
@@ -107,12 +107,6 @@
     <t>Xetra-Gold EUR</t>
   </si>
   <si>
-    <t>Comprar</t>
-  </si>
-  <si>
-    <t>Vender</t>
-  </si>
-  <si>
     <t>FECHA</t>
   </si>
   <si>
@@ -504,6 +498,15 @@
   </si>
   <si>
     <t>SelfBank</t>
+  </si>
+  <si>
+    <t>IE00B4WXT857</t>
+  </si>
+  <si>
+    <t>Compra</t>
+  </si>
+  <si>
+    <t>Venta</t>
   </si>
 </sst>
 </file>
@@ -891,7 +894,7 @@
   <cols>
     <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" bestFit="1" customWidth="1"/>
@@ -907,46 +910,48 @@
     <row r="1" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>125</v>
-      </c>
       <c r="K2" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>153</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E3" s="3">
         <v>44225</v>
@@ -968,19 +973,22 @@
         <v>1000.02</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="str">
+        <f t="shared" ref="C4:C67" si="1">IF(B4="Amundi IS JP Morgan GBI Glbl Gvs AHE-C","LU0389812933",IF(B4="Deka Dt. Boerse EUROGOV® Ger 10+ ETF","DE000ETFL219",IF(B4="Invesco Physical Gold ETC EUR","IE00B579F325",IF(B4="Lyxor Core STOXX Europe 600(DR) ETF Acc EUR","LU0908500753",IF(B4="Vanguard 20+ Yr € Trs Idx € Acc","IE00B246KL88",IF(B4="Vanguard Em Mkts Stk Idx € Acc","IE0031786696",IF(B4="Vanguard Emerg Mkts Stk Idx Inv EUR Acc","IE0031786142",IF(B4="Vanguard European Stock Idx Inv EUR Acc","IE0007987690",IF(B4="Vanguard FTSE All-World ETF USD Acc EUR","IE00BK5BQT80",IF(B4="Vanguard FTSE Dev AsiaPac exJpnETFUSDAcc EUR","IE00BK5BQZ41",IF(B4="Vanguard FTSE Emerg Markets ETF USD Acc EUR","IE00BK5BR733",IF(B4="Vanguard Japan Stock Index Inv EUR Acc","IE0007281425",IF(B4="Vanguard Jpn Stk Idx € Acc","IE0007286036",IF(B4="Vanguard Pac ex-Japan Stk Idx EUR Acc","IE0007201266",IF(B4="Vanguard U.S. 500 Stk Idx € Acc","IE0032126645",IF(B4="Vanguard US 500 Stock Index Inv EUR Acc","IE0032620787",IF(B4="Vanguard €pean Stk Idx € Acc","IE0007987708",IF(B4="Vanguard €z Infl-Lnkd Bd Idx € Acc","IE00B04GQR24",IF(B4="WisdomTree Physical Swiss Gold ETC EUR","DE000A1DCTL3",IF(B4="Xetra-Gold EUR","DE000A0S9GB0",IF(B4="iShares Core MSCI Japan IMI ETF USD Acc EUR","IE00B4L5YX21",IF(B4="iShares Core S&amp;amp;P 500 ETF USD Acc EUR","IE00B5BMR087",IF(B4="iShares Pacific Index (IE) D Acc EUR","IE00BDRK7R97",IF(B4="iShares UltraHQ EurGovtBdIdx(IE)InstAcc€","IE00B4XCK338",IF(B4="iShares eb.rexx® GovtGer 10.5+yr (DE)","DE000A0D8Q31",IF(B4="iShares € Govt Bond 20y TgtDur ETF€ Dist EUR","IE00BSKRJX20","xyz"))))))))))))))))))))))))))</f>
+        <v>IE0007286036</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E4" s="3">
         <v>44225</v>
@@ -1002,19 +1010,22 @@
         <v>1111.53</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007281425</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E5" s="3">
         <v>44225</v>
@@ -1036,19 +1047,22 @@
         <v>1113.8499999999999</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007987708</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E6" s="3">
         <v>44224</v>
@@ -1066,23 +1080,26 @@
         <v>2451.63</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" ref="J6:J37" si="1">ROUND((F6*G6)+H6,2)</f>
+        <f t="shared" ref="J6:J37" si="2">ROUND((F6*G6)+H6,2)</f>
         <v>2451.63</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0032126645</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E7" s="3">
         <v>44224</v>
@@ -1100,23 +1117,26 @@
         <v>2197.89</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2197.89</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007987690</v>
+      </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E8" s="3">
         <v>44224</v>
@@ -1134,23 +1154,26 @@
         <v>2451.69</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2451.69</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0032620787</v>
+      </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E9" s="3">
         <v>44224</v>
@@ -1168,23 +1191,26 @@
         <v>2198.2600000000002</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2198.2600000000002</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B4XCK338</v>
+      </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E10" s="3">
         <v>44221</v>
@@ -1202,23 +1228,26 @@
         <v>999.92</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>999.92</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B04GQR24</v>
+      </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E11" s="3">
         <v>44217</v>
@@ -1236,23 +1265,26 @@
         <v>1047.24</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1047.24</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B579F325</v>
+      </c>
       <c r="D12" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E12" s="3">
         <v>44216</v>
@@ -1270,23 +1302,26 @@
         <v>1484.44</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1484.44</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>LU0389812933</v>
+      </c>
       <c r="D13" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E13" s="3">
         <v>44215</v>
@@ -1304,23 +1339,26 @@
         <v>1047.9100000000001</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1047.9100000000001</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007201266</v>
+      </c>
       <c r="D14" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E14" s="3">
         <v>44200</v>
@@ -1338,23 +1376,26 @@
         <v>1111.6300000000001</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1111.6300000000001</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00BDRK7R97</v>
+      </c>
       <c r="D15" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E15" s="3">
         <v>44197</v>
@@ -1372,23 +1413,26 @@
         <v>1111.6199999999999</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1111.6199999999999</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007281425</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E16" s="3">
         <v>44174</v>
@@ -1406,23 +1450,26 @@
         <v>1063.53</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1063.53</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007286036</v>
+      </c>
       <c r="D17" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E17" s="3">
         <v>44174</v>
@@ -1440,23 +1487,26 @@
         <v>1063.53</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1063.53</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00BDRK7R97</v>
+      </c>
       <c r="D18" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E18" s="3">
         <v>44173</v>
@@ -1474,23 +1524,26 @@
         <v>1116.8699999999999</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1116.8699999999999</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007201266</v>
+      </c>
       <c r="D19" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E19" s="3">
         <v>44173</v>
@@ -1508,23 +1561,26 @@
         <v>1116.8699999999999</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1116.8699999999999</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007987690</v>
+      </c>
       <c r="D20" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E20" s="3">
         <v>44167</v>
@@ -1542,23 +1598,26 @@
         <v>2387.34</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2387.34</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007987708</v>
+      </c>
       <c r="D21" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E21" s="3">
         <v>44166</v>
@@ -1576,23 +1635,26 @@
         <v>2387.35</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2387.35</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0032620787</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E22" s="3">
         <v>44161</v>
@@ -1610,23 +1672,26 @@
         <v>2154.88</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2154.88</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0032126645</v>
+      </c>
       <c r="D23" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E23" s="3">
         <v>44160</v>
@@ -1644,23 +1709,26 @@
         <v>2154.88</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2154.88</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0031786142</v>
+      </c>
       <c r="D24" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E24" s="3">
         <v>44159</v>
@@ -1678,23 +1746,26 @@
         <v>2200.3000000000002</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2200.3000000000002</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0031786696</v>
+      </c>
       <c r="D25" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E25" s="3">
         <v>44158</v>
@@ -1712,23 +1783,26 @@
         <v>2200.3000000000002</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2200.3000000000002</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0031786696</v>
+      </c>
       <c r="D26" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E26" s="3">
         <v>44141</v>
@@ -1746,23 +1820,26 @@
         <v>681.15</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>681.15</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0032126645</v>
+      </c>
       <c r="D27" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E27" s="3">
         <v>44140</v>
@@ -1780,23 +1857,26 @@
         <v>681.75</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>681.75</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B246KL88</v>
+      </c>
       <c r="D28" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E28" s="3">
         <v>44138</v>
@@ -1814,23 +1894,26 @@
         <v>975.79</v>
       </c>
       <c r="J28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>975.79</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B246KL88</v>
+      </c>
       <c r="D29" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E29" s="3">
         <v>44138</v>
@@ -1848,23 +1931,26 @@
         <v>942.9</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>942.9</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007987708</v>
+      </c>
       <c r="D30" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E30" s="3">
         <v>44138</v>
@@ -1882,23 +1968,26 @@
         <v>799.93</v>
       </c>
       <c r="J30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>799.93</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B4XCK338</v>
+      </c>
       <c r="D31" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E31" s="3">
         <v>44137</v>
@@ -1916,23 +2005,26 @@
         <v>976.81</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>976.81</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>LU0389812933</v>
+      </c>
       <c r="D32" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E32" s="3">
         <v>44137</v>
@@ -1950,23 +2042,26 @@
         <v>944.19</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>944.19</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B4XCK338</v>
+      </c>
       <c r="D33" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E33" s="3">
         <v>44132</v>
@@ -1984,23 +2079,26 @@
         <v>1996.65</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1996.65</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="2"/>
+      <c r="C34" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>LU0389812933</v>
+      </c>
       <c r="D34" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E34" s="3">
         <v>44131</v>
@@ -2018,23 +2116,26 @@
         <v>1999.9</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1999.9</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="2"/>
+      <c r="C35" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B246KL88</v>
+      </c>
       <c r="D35" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E35" s="3">
         <v>44131</v>
@@ -2052,23 +2153,26 @@
         <v>998.85</v>
       </c>
       <c r="J35" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>998.85</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="2"/>
+      <c r="C36" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DE000A0D8Q31</v>
+      </c>
       <c r="D36" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E36" s="3">
         <v>44131</v>
@@ -2086,23 +2190,26 @@
         <v>2948.31</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2954.09</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="2"/>
+      <c r="C37" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DE000A1DCTL3</v>
+      </c>
       <c r="D37" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E37" s="3">
         <v>44127</v>
@@ -2120,23 +2227,26 @@
         <v>4835.5</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4835.5</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="2"/>
+      <c r="C38" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DE000A1DCTL3</v>
+      </c>
       <c r="D38" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E38" s="3">
         <v>44127</v>
@@ -2154,23 +2264,26 @@
         <v>2955.64</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" ref="J38:J73" si="2">ROUND((F38*G38)+H38,2)</f>
+        <f t="shared" ref="J38:J73" si="3">ROUND((F38*G38)+H38,2)</f>
         <v>2955.64</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="2"/>
+      <c r="C39" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DE000A0D8Q31</v>
+      </c>
       <c r="D39" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E39" s="3">
         <v>44118</v>
@@ -2188,23 +2301,26 @@
         <v>839.21</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>839.21</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="2"/>
+      <c r="C40" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B246KL88</v>
+      </c>
       <c r="D40" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E40" s="3">
         <v>44118</v>
@@ -2222,23 +2338,26 @@
         <v>909.45</v>
       </c>
       <c r="J40" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>914.39</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="2"/>
+      <c r="C41" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0031786696</v>
+      </c>
       <c r="D41" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E41" s="3">
         <v>44112</v>
@@ -2256,23 +2375,26 @@
         <v>1349.49</v>
       </c>
       <c r="J41" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1349.49</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="2"/>
+      <c r="C42" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B246KL88</v>
+      </c>
       <c r="D42" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E42" s="3">
         <v>44112</v>
@@ -2290,23 +2412,26 @@
         <v>1004.49</v>
       </c>
       <c r="J42" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1004.49</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="2"/>
+      <c r="C43" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B4XCK338</v>
+      </c>
       <c r="D43" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E43" s="3">
         <v>44112</v>
@@ -2324,23 +2449,26 @@
         <v>1007.08</v>
       </c>
       <c r="J43" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1007.08</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="2"/>
+      <c r="C44" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0032126645</v>
+      </c>
       <c r="D44" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E44" s="3">
         <v>44110</v>
@@ -2358,23 +2486,26 @@
         <v>294.95999999999998</v>
       </c>
       <c r="J44" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>294.95999999999998</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="2"/>
+      <c r="C45" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007987708</v>
+      </c>
       <c r="D45" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E45" s="3">
         <v>44110</v>
@@ -2392,23 +2523,26 @@
         <v>350</v>
       </c>
       <c r="J45" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>350</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="2"/>
+      <c r="C46" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00BK5BR733</v>
+      </c>
       <c r="D46" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E46" s="3">
         <v>44106</v>
@@ -2426,23 +2560,26 @@
         <v>1013.88</v>
       </c>
       <c r="J46" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1018.48</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="2"/>
+      <c r="C47" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00BK5BQZ41</v>
+      </c>
       <c r="D47" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E47" s="3">
         <v>44106</v>
@@ -2460,23 +2597,26 @@
         <v>1008.44</v>
       </c>
       <c r="J47" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1013.04</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C48" s="2"/>
+      <c r="C48" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B4L5YX21</v>
+      </c>
       <c r="D48" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E48" s="3">
         <v>44106</v>
@@ -2494,23 +2634,26 @@
         <v>1016.13</v>
       </c>
       <c r="J48" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1020.75</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="2"/>
+      <c r="C49" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007286036</v>
+      </c>
       <c r="D49" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E49" s="3">
         <v>44105</v>
@@ -2528,23 +2671,26 @@
         <v>1000.59</v>
       </c>
       <c r="J49" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1000.59</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="2"/>
+      <c r="C50" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007201266</v>
+      </c>
       <c r="D50" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E50" s="3">
         <v>44105</v>
@@ -2562,23 +2708,26 @@
         <v>999.41</v>
       </c>
       <c r="J50" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>999.41</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="2"/>
+      <c r="C51" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0032126645</v>
+      </c>
       <c r="D51" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E51" s="3">
         <v>44104</v>
@@ -2596,23 +2745,26 @@
         <v>1064.49</v>
       </c>
       <c r="J51" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1064.49</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="2"/>
+      <c r="C52" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B5BMR087</v>
+      </c>
       <c r="D52" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E52" s="3">
         <v>44104</v>
@@ -2630,23 +2782,26 @@
         <v>1139.2</v>
       </c>
       <c r="J52" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1139.2</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="2"/>
+      <c r="C53" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE0007987708</v>
+      </c>
       <c r="D53" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E53" s="3">
         <v>44099</v>
@@ -2664,23 +2819,26 @@
         <v>1000.02</v>
       </c>
       <c r="J53" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1000.02</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C54" s="2"/>
+      <c r="C54" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>LU0908500753</v>
+      </c>
       <c r="D54" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E54" s="3">
         <v>44099</v>
@@ -2698,23 +2856,26 @@
         <v>1029.49</v>
       </c>
       <c r="J54" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1034.1099999999999</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="2"/>
+      <c r="C55" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B246KL88</v>
+      </c>
       <c r="D55" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E55" s="3">
         <v>44098</v>
@@ -2732,23 +2893,26 @@
         <v>3991.84</v>
       </c>
       <c r="J55" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3991.84</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="2"/>
+      <c r="C56" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DE000A1DCTL3</v>
+      </c>
       <c r="D56" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E56" s="3">
         <v>44098</v>
@@ -2766,23 +2930,26 @@
         <v>2926.95</v>
       </c>
       <c r="J56" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2926.95</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C57" s="2"/>
+      <c r="C57" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00BSKRJX20</v>
+      </c>
       <c r="D57" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E57" s="3">
         <v>44098</v>
@@ -2800,23 +2967,26 @@
         <v>1030.75</v>
       </c>
       <c r="J57" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1035.3699999999999</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="2"/>
+      <c r="C58" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DE000ETFL219</v>
+      </c>
       <c r="D58" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E58" s="3">
         <v>44098</v>
@@ -2834,23 +3004,26 @@
         <v>1952.88</v>
       </c>
       <c r="J58" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1958.06</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="2"/>
+      <c r="C59" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B246KL88</v>
+      </c>
       <c r="D59" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E59" s="3">
         <v>44098</v>
@@ -2868,23 +3041,26 @@
         <v>1064.49</v>
       </c>
       <c r="J59" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1064.49</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C60" s="2"/>
+      <c r="C60" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B4XCK338</v>
+      </c>
       <c r="D60" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E60" s="3">
         <v>44092</v>
@@ -2902,23 +3078,26 @@
         <v>1005.63</v>
       </c>
       <c r="J60" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1005.63</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C61" s="2"/>
+      <c r="C61" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00BSKRJX20</v>
+      </c>
       <c r="D61" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E61" s="3">
         <v>44020</v>
@@ -2936,23 +3115,26 @@
         <v>1014.11</v>
       </c>
       <c r="J61" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1014.11</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C62" s="2"/>
+      <c r="C62" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00BK5BR733</v>
+      </c>
       <c r="D62" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E62" s="3">
         <v>44020</v>
@@ -2970,23 +3152,26 @@
         <v>1047.53</v>
       </c>
       <c r="J62" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1047.53</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="2"/>
+      <c r="C63" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00BK5BQZ41</v>
+      </c>
       <c r="D63" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E63" s="3">
         <v>44020</v>
@@ -3004,23 +3189,26 @@
         <v>1021.27</v>
       </c>
       <c r="J63" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1021.27</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C64" s="2"/>
+      <c r="C64" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>LU0908500753</v>
+      </c>
       <c r="D64" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E64" s="3">
         <v>43998</v>
@@ -3038,23 +3226,26 @@
         <v>1062.82</v>
       </c>
       <c r="J64" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1062.82</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C65" s="2"/>
+      <c r="C65" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DE000ETFL219</v>
+      </c>
       <c r="D65" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E65" s="3">
         <v>43998</v>
@@ -3072,23 +3263,26 @@
         <v>1046.25</v>
       </c>
       <c r="J65" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1046.25</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C66" s="2"/>
+      <c r="C66" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DE000A0D8Q31</v>
+      </c>
       <c r="D66" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E66" s="3">
         <v>43998</v>
@@ -3106,23 +3300,26 @@
         <v>1017.05</v>
       </c>
       <c r="J66" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1017.05</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B67" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C67" s="2"/>
+      <c r="C67" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>IE00B4L5YX21</v>
+      </c>
       <c r="D67" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E67" s="3">
         <v>43998</v>
@@ -3140,23 +3337,26 @@
         <v>1017.1</v>
       </c>
       <c r="J67" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1017.1</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B68" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="2"/>
+      <c r="C68" s="2" t="str">
+        <f t="shared" ref="C68:C73" si="4">IF(B68="Amundi IS JP Morgan GBI Glbl Gvs AHE-C","LU0389812933",IF(B68="Deka Dt. Boerse EUROGOV® Ger 10+ ETF","DE000ETFL219",IF(B68="Invesco Physical Gold ETC EUR","IE00B579F325",IF(B68="Lyxor Core STOXX Europe 600(DR) ETF Acc EUR","LU0908500753",IF(B68="Vanguard 20+ Yr € Trs Idx € Acc","IE00B246KL88",IF(B68="Vanguard Em Mkts Stk Idx € Acc","IE0031786696",IF(B68="Vanguard Emerg Mkts Stk Idx Inv EUR Acc","IE0031786142",IF(B68="Vanguard European Stock Idx Inv EUR Acc","IE0007987690",IF(B68="Vanguard FTSE All-World ETF USD Acc EUR","IE00BK5BQT80",IF(B68="Vanguard FTSE Dev AsiaPac exJpnETFUSDAcc EUR","IE00BK5BQZ41",IF(B68="Vanguard FTSE Emerg Markets ETF USD Acc EUR","IE00BK5BR733",IF(B68="Vanguard Japan Stock Index Inv EUR Acc","IE0007281425",IF(B68="Vanguard Jpn Stk Idx € Acc","IE0007286036",IF(B68="Vanguard Pac ex-Japan Stk Idx EUR Acc","IE0007201266",IF(B68="Vanguard U.S. 500 Stk Idx € Acc","IE0032126645",IF(B68="Vanguard US 500 Stock Index Inv EUR Acc","IE0032620787",IF(B68="Vanguard €pean Stk Idx € Acc","IE0007987708",IF(B68="Vanguard €z Infl-Lnkd Bd Idx € Acc","IE00B04GQR24",IF(B68="WisdomTree Physical Swiss Gold ETC EUR","DE000A1DCTL3",IF(B68="Xetra-Gold EUR","DE000A0S9GB0",IF(B68="iShares Core MSCI Japan IMI ETF USD Acc EUR","IE00B4L5YX21",IF(B68="iShares Core S&amp;amp;P 500 ETF USD Acc EUR","IE00B5BMR087",IF(B68="iShares Pacific Index (IE) D Acc EUR","IE00BDRK7R97",IF(B68="iShares UltraHQ EurGovtBdIdx(IE)InstAcc€","IE00B4XCK338",IF(B68="iShares eb.rexx® GovtGer 10.5+yr (DE)","DE000A0D8Q31",IF(B68="iShares € Govt Bond 20y TgtDur ETF€ Dist EUR","IE00BSKRJX20","xyz"))))))))))))))))))))))))))</f>
+        <v>IE00B5BMR087</v>
+      </c>
       <c r="D68" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E68" s="3">
         <v>43998</v>
@@ -3174,23 +3374,26 @@
         <v>1118.3699999999999</v>
       </c>
       <c r="J68" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1118.3699999999999</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B69" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C69" s="2"/>
+      <c r="C69" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>IE00BK5BQT80</v>
+      </c>
       <c r="D69" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E69" s="3">
         <v>43998</v>
@@ -3208,23 +3411,26 @@
         <v>942.17</v>
       </c>
       <c r="J69" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>946.73</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B70" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C70" s="2"/>
+      <c r="C70" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>IE00BK5BQT80</v>
+      </c>
       <c r="D70" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E70" s="3">
         <v>43992</v>
@@ -3242,23 +3448,26 @@
         <v>960</v>
       </c>
       <c r="J70" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>960</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B71" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C71" s="2"/>
+      <c r="C71" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>DE000A0D8Q31</v>
+      </c>
       <c r="D71" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E71" s="3">
         <v>43991</v>
@@ -3276,23 +3485,26 @@
         <v>1000.48</v>
       </c>
       <c r="J71" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1000.48</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B72" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C72" s="2"/>
+      <c r="C72" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>DE000ETFL219</v>
+      </c>
       <c r="D72" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E72" s="3">
         <v>43991</v>
@@ -3310,23 +3522,26 @@
         <v>857.36</v>
       </c>
       <c r="J72" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>857.36</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B73" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C73" s="2"/>
+      <c r="C73" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>DE000A0S9GB0</v>
+      </c>
       <c r="D73" s="2" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="E73" s="3">
         <v>43991</v>
@@ -3344,14 +3559,14 @@
         <v>2985.7</v>
       </c>
       <c r="J73" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2985.7</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3386,31 +3601,31 @@
     <row r="1" spans="2:10" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="J2" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
@@ -3418,28 +3633,28 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="J3" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
@@ -3447,28 +3662,28 @@
         <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="J4" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
@@ -3476,28 +3691,28 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="J5" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
@@ -3505,28 +3720,28 @@
         <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
@@ -3534,28 +3749,28 @@
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
@@ -3563,28 +3778,28 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -3592,28 +3807,28 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
@@ -3621,28 +3836,28 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
@@ -3650,28 +3865,28 @@
         <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
@@ -3679,28 +3894,28 @@
         <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
@@ -3708,28 +3923,28 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
@@ -3737,28 +3952,28 @@
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
@@ -3766,28 +3981,28 @@
         <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
@@ -3795,28 +4010,28 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
@@ -3824,28 +4039,28 @@
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
@@ -3853,28 +4068,28 @@
         <v>10</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
@@ -3882,28 +4097,28 @@
         <v>9</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
@@ -3911,28 +4126,28 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
@@ -3940,28 +4155,28 @@
         <v>16</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="J21" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
@@ -3969,28 +4184,28 @@
         <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="J22" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
@@ -3998,28 +4213,28 @@
         <v>19</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
@@ -4027,28 +4242,28 @@
         <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
@@ -4056,28 +4271,28 @@
         <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
@@ -4085,28 +4300,28 @@
         <v>0</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J26" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
@@ -4114,28 +4329,28 @@
         <v>15</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="J27" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
@@ -4143,28 +4358,28 @@
         <v>22</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="J28" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -4223,19 +4438,19 @@
     <row r="1" spans="2:6" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
@@ -4243,7 +4458,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2">
         <v>144.43</v>
@@ -4258,7 +4473,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2">
         <v>176.97</v>
@@ -4273,7 +4488,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2">
         <v>147.72999999999999</v>
@@ -4288,7 +4503,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2">
         <v>171.12</v>
@@ -4303,7 +4518,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D7" s="2">
         <v>269.13</v>
@@ -4318,7 +4533,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D8" s="2">
         <v>212.2</v>
@@ -4333,7 +4548,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D9" s="2">
         <v>210.77</v>
@@ -4348,7 +4563,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10" s="2">
         <v>22.14</v>
@@ -4363,7 +4578,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D11" s="2">
         <v>84.89</v>
@@ -4378,7 +4593,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D12" s="2">
         <v>27.46</v>
@@ -4393,7 +4608,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13" s="2">
         <v>56.09</v>
@@ -4408,7 +4623,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D14" s="2">
         <v>229.97</v>
@@ -4423,7 +4638,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D15" s="2">
         <v>230.91</v>
@@ -4438,7 +4653,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D16" s="2">
         <v>247.12</v>
@@ -4453,7 +4668,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D17" s="2">
         <v>36.68</v>
@@ -4468,7 +4683,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D18" s="2">
         <v>35.94</v>
@@ -4483,7 +4698,7 @@
         <v>9</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D19" s="2">
         <v>22.57</v>
@@ -4498,7 +4713,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D20" s="2">
         <v>133.82</v>
@@ -4513,7 +4728,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D21" s="2">
         <v>147</v>
@@ -4528,7 +4743,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D22" s="2">
         <v>49.04</v>
@@ -4543,7 +4758,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D23" s="2">
         <v>42.88</v>
@@ -4558,7 +4773,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D24" s="2">
         <v>319.94</v>
@@ -4573,7 +4788,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D25" s="2">
         <v>12.38</v>
@@ -4588,7 +4803,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D26" s="2">
         <v>13.29</v>
@@ -4603,7 +4818,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D27" s="2">
         <v>207.4</v>
@@ -4618,7 +4833,7 @@
         <v>22</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D28" s="2">
         <v>6.53</v>
@@ -4662,212 +4877,212 @@
     <row r="1" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>132</v>
-      </c>
       <c r="H2" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>141</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E22" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="I22" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="J22" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="K22" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>151</v>
-      </c>
       <c r="L22" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>151</v>
-      </c>
       <c r="G24" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>